<commit_message>
conjoint country x vote
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/program_preferred_by_cut_aid_in_program.xlsx
+++ b/xlsx/country_comparison/program_preferred_by_cut_aid_in_program.xlsx
@@ -407,13 +407,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.0553937931714483</v>
+        <v>-0.0405101384793125</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.0778365291031607</v>
+        <v>-0.0643051395617496</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.032951057239736</v>
+        <v>-0.0167151373968755</v>
       </c>
     </row>
     <row r="3">
@@ -421,13 +421,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0568171395511542</v>
+        <v>-0.0395525406328933</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0891148683204101</v>
+        <v>-0.0736720078149598</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.0245194107818982</v>
+        <v>-0.00543307345082682</v>
       </c>
     </row>
     <row r="4">
@@ -435,13 +435,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>0.022834116958244</v>
+        <v>0.0252544925943794</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0577299586936083</v>
+        <v>-0.0598679690449487</v>
       </c>
       <c r="D4" t="n">
-        <v>0.103398192610096</v>
+        <v>0.110376954233708</v>
       </c>
     </row>
     <row r="5">
@@ -449,13 +449,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.0939184481506937</v>
+        <v>-0.0765248032469395</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.161951501120431</v>
+        <v>-0.148482662821163</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0258853951809561</v>
+        <v>-0.004566943672716</v>
       </c>
     </row>
     <row r="6">
@@ -463,13 +463,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.17370172563329</v>
+        <v>-0.171200400434677</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.250128016385663</v>
+        <v>-0.252797961937622</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0972754348809171</v>
+        <v>-0.0896028389317323</v>
       </c>
     </row>
     <row r="7">
@@ -477,13 +477,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.112843680712125</v>
+        <v>-0.0937905063089196</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.21030116511403</v>
+        <v>-0.197428467420491</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0153861963102188</v>
+        <v>0.00984745480265203</v>
       </c>
     </row>
     <row r="8">
@@ -491,13 +491,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.0404812496369166</v>
+        <v>0.00503032067922172</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.130309288116866</v>
+        <v>-0.0896479045450339</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0493467888430328</v>
+        <v>0.0997085459034773</v>
       </c>
     </row>
     <row r="9">
@@ -505,13 +505,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0191721690712545</v>
+        <v>0.0434352917667326</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0603615840597693</v>
+        <v>-0.0399376672538099</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0987059222022782</v>
+        <v>0.126808250787275</v>
       </c>
     </row>
     <row r="10">
@@ -519,13 +519,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0583638302707828</v>
+        <v>0.0845158701934025</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0512298000135148</v>
+        <v>-0.030081917545833</v>
       </c>
       <c r="D10" t="n">
-        <v>0.16795746055508</v>
+        <v>0.199113657932638</v>
       </c>
     </row>
     <row r="11">
@@ -533,13 +533,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0184264255454356</v>
+        <v>-0.00527322075229465</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0677962933855345</v>
+        <v>-0.0576177795886535</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0309434422946632</v>
+        <v>0.0470713380840642</v>
       </c>
     </row>
     <row r="12">
@@ -547,13 +547,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.066834616836694</v>
+        <v>-0.0530237098185993</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.105377543224187</v>
+        <v>-0.0941783085364134</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.0282916904492011</v>
+        <v>-0.0118691111007853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>